<commit_message>
add tabla despues casi todo
</commit_message>
<xml_diff>
--- a/simil_new_numbers.xlsx
+++ b/simil_new_numbers.xlsx
@@ -451,17 +451,17 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Dispositivo COS</t>
+          <t>Dispositivo DAAS</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Puerto COS</t>
+          <t>Puerto DAAS</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>ptp</t>
+          <t>Unnamed: 5</t>
         </is>
       </c>
     </row>

</xml_diff>